<commit_message>
Updated powerlaw fit excel
</commit_message>
<xml_diff>
--- a/powerlaw fit.xlsx
+++ b/powerlaw fit.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhpayne/Documents/GitHub/ASTR6880Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\pegriffin\HighEnergy\ASTR6880Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E140DCB3-2656-9A4E-86AE-CAAA24CB7C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88AC9C8-E3F7-47BA-A8FC-873CCCF899FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="32000" windowHeight="16000"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="obsids" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Epoch</t>
   </si>
@@ -81,12 +81,48 @@
   <si>
     <t>lb</t>
   </si>
+  <si>
+    <t>log(flux)</t>
+  </si>
+  <si>
+    <t>log(time)</t>
+  </si>
+  <si>
+    <t>rsq</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>slope</t>
+  </si>
+  <si>
+    <t>y-int</t>
+  </si>
+  <si>
+    <t>errors</t>
+  </si>
+  <si>
+    <t>Without Epoch 11</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>With all points</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -569,9 +605,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -1043,7 +1078,444 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.31024256342957129"/>
+                  <c:y val="-0.38773366870807818"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>obsids!$L$4:$L$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>2.4158440903765532</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5552849503590882</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.765523278968232</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8705239192769385</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.9727327702650714</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0836138171760776</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0986089175296634</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.1975515440647775</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.2310518996557538</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.3036987100051172</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>obsids!$K$4:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>-13.88941028970075</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-14.110698297493689</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-14.552841968657781</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-14.694648630553376</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-14.866461091629782</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-14.605548319173783</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-15.073143291050307</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-15.369572124974976</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-15.642065152999546</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-15.692503962086787</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-872C-435F-A90F-F7ECD707716A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1935437568"/>
+        <c:axId val="1935438048"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1935437568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1935438048"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1935438048"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1935437568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1599,20 +2071,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>3486150</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>3854450</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1632,6 +2620,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>271462</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>652462</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8B3B386-A3A1-5467-1667-046990B8D2D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1936,19 +2960,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="6" max="6" width="55.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1976,8 +3000,14 @@
       <c r="I1" t="s">
         <v>19</v>
       </c>
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>4</v>
       </c>
@@ -1996,17 +3026,31 @@
       <c r="F2" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>2.3200000000000001E-14</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>2.5199999999999999E-14</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2" s="2">
         <v>2.1300000000000001E-14</v>
       </c>
+      <c r="K2">
+        <f>LOG(G2:G13)</f>
+        <v>-13.634512015109101</v>
+      </c>
+      <c r="L2">
+        <f>LOG(C2)</f>
+        <v>2.0410544336692147</v>
+      </c>
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>5</v>
       </c>
@@ -2025,17 +3069,32 @@
       <c r="F3" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>2.3999999999999999E-14</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>2.5899999999999999E-14</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3" s="2">
         <v>2.2000000000000001E-14</v>
       </c>
+      <c r="K3">
+        <f>LOG(G3:G14)</f>
+        <v>-13.619788758288394</v>
+      </c>
+      <c r="L3">
+        <f>LOG(C3)</f>
+        <v>2.2017531188589214</v>
+      </c>
+      <c r="O3">
+        <f t="array" ref="O3:P5">LINEST(K4:K13,L4:L13,TRUE,TRUE)</f>
+        <v>-1.9334270841585413</v>
+      </c>
+      <c r="P3">
+        <v>-9.1471555798627779</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>6</v>
       </c>
@@ -2054,18 +3113,34 @@
       <c r="F4" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>1.2900000000000001E-14</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>1.4500000000000001E-14</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4" s="2">
         <v>1.1400000000000001E-14</v>
       </c>
-      <c r="K4" s="1"/>
+      <c r="K4">
+        <f>LOG(G4:G15)</f>
+        <v>-13.88941028970075</v>
+      </c>
+      <c r="L4">
+        <f>LOG(C4)</f>
+        <v>2.4158440903765532</v>
+      </c>
+      <c r="N4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4">
+        <v>0.23763368633397353</v>
+      </c>
+      <c r="P4">
+        <v>0.70405154519407009</v>
+      </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>7</v>
       </c>
@@ -2084,17 +3159,31 @@
       <c r="F5">
         <v>21371</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>7.7500000000000001E-15</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>9.3100000000000002E-15</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="2">
         <v>6.3699999999999998E-15</v>
       </c>
+      <c r="K5">
+        <f>LOG(G5:G16)</f>
+        <v>-14.110698297493689</v>
+      </c>
+      <c r="L5">
+        <f>LOG(C5)</f>
+        <v>2.5552849503590882</v>
+      </c>
+      <c r="O5">
+        <v>0.89217921211503481</v>
+      </c>
+      <c r="P5">
+        <v>0.21085169795001729</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>8</v>
       </c>
@@ -2113,17 +3202,25 @@
       <c r="F6" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>2.8000000000000001E-15</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>3.6600000000000003E-15</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="2">
         <v>2.0599999999999999E-15</v>
       </c>
+      <c r="K6">
+        <f>LOG(G6:G17)</f>
+        <v>-14.552841968657781</v>
+      </c>
+      <c r="L6">
+        <f>LOG(C6)</f>
+        <v>2.765523278968232</v>
+      </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>9</v>
       </c>
@@ -2142,17 +3239,29 @@
       <c r="F7" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="2">
         <v>2.0200000000000001E-15</v>
       </c>
-      <c r="H7" s="3">
+      <c r="H7" s="2">
         <v>2.8000000000000001E-15</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="2">
         <v>1.37E-15</v>
       </c>
+      <c r="K7">
+        <f>LOG(G7:G18)</f>
+        <v>-14.694648630553376</v>
+      </c>
+      <c r="L7">
+        <f>LOG(C7)</f>
+        <v>2.8705239192769385</v>
+      </c>
+      <c r="O7">
+        <f>O3-O4</f>
+        <v>-2.1710607704925149</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>10</v>
       </c>
@@ -2171,17 +3280,25 @@
       <c r="F8" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>1.36E-15</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>2.0799999999999999E-15</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="2">
         <v>7.7399999999999996E-16</v>
       </c>
+      <c r="K8">
+        <f>LOG(G8:G19)</f>
+        <v>-14.866461091629782</v>
+      </c>
+      <c r="L8">
+        <f>LOG(C8)</f>
+        <v>2.9727327702650714</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>11</v>
       </c>
@@ -2200,17 +3317,25 @@
       <c r="F9" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>2.4800000000000001E-15</v>
       </c>
-      <c r="H9" s="3">
+      <c r="H9" s="2">
         <v>3.4300000000000001E-15</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="2">
         <v>1.6800000000000001E-15</v>
       </c>
+      <c r="K9">
+        <f t="shared" ref="K9:K13" si="0">LOG(G9:G20)</f>
+        <v>-14.605548319173783</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ref="L9:L13" si="1">LOG(C9)</f>
+        <v>3.0836138171760776</v>
+      </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>12</v>
       </c>
@@ -2229,17 +3354,25 @@
       <c r="F10" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>8.4500000000000002E-16</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>1.47E-15</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="2">
         <v>3.3599999999999999E-16</v>
       </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>-15.073143291050307</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>3.0986089175296634</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>13</v>
       </c>
@@ -2258,17 +3391,25 @@
       <c r="F11" t="s">
         <v>14</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>4.2699999999999999E-16</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H11" s="2">
         <v>9.1200000000000003E-16</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="2">
         <v>5.2800000000000003E-17</v>
       </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>-15.369572124974976</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="1"/>
+        <v>3.1975515440647775</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>14</v>
       </c>
@@ -2287,17 +3428,28 @@
       <c r="F12" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>2.2800000000000001E-16</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>7.0500000000000002E-16</v>
       </c>
       <c r="I12">
         <v>0</v>
       </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>-15.642065152999546</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="1"/>
+        <v>3.2310518996557538</v>
+      </c>
+      <c r="O12" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>15</v>
       </c>
@@ -2316,14 +3468,77 @@
       <c r="F13" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>2.03E-16</v>
       </c>
-      <c r="H13" s="3">
+      <c r="H13" s="2">
         <v>5.2499999999999995E-16</v>
       </c>
       <c r="I13">
         <v>0</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>-15.692503962086787</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="1"/>
+        <v>3.3036987100051172</v>
+      </c>
+      <c r="N13" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13">
+        <v>-1.9334270841585413</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="N14" t="s">
+        <v>31</v>
+      </c>
+      <c r="O14">
+        <v>0.23763368633397353</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="M15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="M16">
+        <v>0.89219999999999999</v>
+      </c>
+      <c r="P16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="13:16">
+      <c r="M17" t="s">
+        <v>23</v>
+      </c>
+      <c r="P17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="13:16">
+      <c r="M18">
+        <f>SQRT(M16)</f>
+        <v>0.94456339120251742</v>
+      </c>
+      <c r="O18" t="s">
+        <v>28</v>
+      </c>
+      <c r="P18">
+        <v>-2.0312621735276362</v>
+      </c>
+    </row>
+    <row r="19" spans="13:16">
+      <c r="O19" t="s">
+        <v>29</v>
+      </c>
+      <c r="P19">
+        <v>0.11134367972126213</v>
       </c>
     </row>
   </sheetData>

</xml_diff>